<commit_message>
Biomass data for LE20 updated using new data from Ian Broad.
</commit_message>
<xml_diff>
--- a/Tests/Validation/DCaPST/Sorghum/obs/Observed.xlsx
+++ b/Tests/Validation/DCaPST/Sorghum/obs/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ApsimX\Tests\UnderReview\Sorghum\obs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apsim\ApsimQaafi\Tests\Validation\Sorghum\obs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F136BB8-107F-467A-85AC-27DBFCC3C784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA7AB2-7F31-460B-B1F3-D58E9BF7761D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2385" windowWidth="29775" windowHeight="16365" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5775" yWindow="270" windowWidth="21600" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -589,8 +589,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,9 +610,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -649,7 +650,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -755,7 +756,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -897,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -911,14 +912,17 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomRight" activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
     <col min="40" max="40" width="11.28515625" customWidth="1"/>
     <col min="42" max="42" width="11.5703125" customWidth="1"/>
   </cols>
@@ -8426,25 +8430,31 @@
         <v>163</v>
       </c>
       <c r="D84">
-        <v>13501.990000000002</v>
-      </c>
-      <c r="F84">
-        <v>27.5</v>
-      </c>
-      <c r="I84">
-        <v>809.89300000000003</v>
-      </c>
-      <c r="J84">
-        <v>0.6</v>
-      </c>
-      <c r="M84">
-        <v>1350.1990000000001</v>
-      </c>
-      <c r="O84">
+        <f>M84*10</f>
+        <v>16210.916837641551</v>
+      </c>
+      <c r="F84" s="1">
+        <v>32.048986644503337</v>
+      </c>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>920.05</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0.5675496390578324</v>
+      </c>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1">
+        <v>1621.0916837641551</v>
+      </c>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1">
         <v>3.2450000000000001</v>
       </c>
       <c r="AA84">
-        <v>29475.940999999999</v>
+        <v>28707.615944474674</v>
       </c>
       <c r="AN84">
         <v>10</v>
@@ -8467,25 +8477,31 @@
         <v>167</v>
       </c>
       <c r="D85">
-        <v>11740.59</v>
-      </c>
-      <c r="F85">
-        <v>27.2</v>
-      </c>
-      <c r="I85">
-        <v>703.98500000000001</v>
-      </c>
-      <c r="J85">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="M85">
-        <v>1174.059</v>
-      </c>
-      <c r="O85">
+        <f t="shared" ref="D85:D87" si="0">M85*10</f>
+        <v>18541.640484367974</v>
+      </c>
+      <c r="F85" s="1">
+        <v>28.667106561862337</v>
+      </c>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>1046.2033333333334</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0.56424529114096622</v>
+      </c>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1">
+        <v>1854.1640484367974</v>
+      </c>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1">
         <v>4.673</v>
       </c>
       <c r="AA85">
-        <v>24853.808000000001</v>
+        <v>36494.905095345894</v>
       </c>
       <c r="AN85">
         <v>10</v>
@@ -8508,25 +8524,31 @@
         <v>168</v>
       </c>
       <c r="D86">
-        <v>21823.989999999998</v>
-      </c>
-      <c r="F86">
-        <v>28.167000000000002</v>
-      </c>
-      <c r="I86">
-        <v>1280.6890000000001</v>
-      </c>
-      <c r="J86">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="M86">
-        <v>2182.3989999999999</v>
-      </c>
-      <c r="O86">
+        <f t="shared" si="0"/>
+        <v>20620.383238726768</v>
+      </c>
+      <c r="F86" s="1">
+        <v>28.004261301873328</v>
+      </c>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1">
+        <v>1072.5766666666666</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0.52015360444527525</v>
+      </c>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1">
+        <v>2062.0383238726768</v>
+      </c>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1">
         <v>5.4340000000000002</v>
       </c>
       <c r="AA86">
-        <v>46217.048999999999</v>
+        <v>38300.480598462251</v>
       </c>
       <c r="AN86">
         <v>10</v>
@@ -8549,25 +8571,31 @@
         <v>169</v>
       </c>
       <c r="D87">
-        <v>16543.36</v>
-      </c>
-      <c r="F87">
-        <v>22.582999999999998</v>
-      </c>
-      <c r="I87">
-        <v>856.49900000000002</v>
-      </c>
-      <c r="J87">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="M87">
-        <v>1654.336</v>
-      </c>
-      <c r="O87">
+        <f t="shared" si="0"/>
+        <v>18544.689953172063</v>
+      </c>
+      <c r="F87" s="1">
+        <v>24.557108460546885</v>
+      </c>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1">
+        <v>923.85</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0.4981749505291545</v>
+      </c>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1">
+        <v>1854.4689953172062</v>
+      </c>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1">
         <v>5.7430000000000003</v>
       </c>
       <c r="AA87">
-        <v>39483.338000000003</v>
+        <v>37620.471542252002</v>
       </c>
       <c r="AN87">
         <v>10</v>

</xml_diff>